<commit_message>
fixed graph in excel for mtcars
</commit_message>
<xml_diff>
--- a/Misc/CarsSimpleReg.xlsx
+++ b/Misc/CarsSimpleReg.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>mpg (y)</t>
   </si>
@@ -190,7 +190,7 @@
     <t>Residualstandardavvikelse</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>s_e</t>
   </si>
   <si>
     <t xml:space="preserve">R² = SSR/SST = </t>
@@ -202,13 +202,16 @@
     <t>n</t>
   </si>
   <si>
+    <t>t^2 = F vid ENKEL linjär regression (check ok!)</t>
+  </si>
+  <si>
     <t>r^2 = R² (check ok!)</t>
   </si>
   <si>
     <t>df = n-2</t>
   </si>
   <si>
-    <t>t0.975(30)</t>
+    <t>t_0.975(30)</t>
   </si>
 </sst>
 </file>
@@ -325,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -382,6 +385,7 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="10" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="11" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -418,7 +422,7 @@
                 </a:solidFill>
                 <a:latin typeface="Roboto"/>
               </a:rPr>
-              <a:t>hp (x) vs. mpg (y)</a:t>
+              <a:t>mtcars</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -435,7 +439,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>mtcars!$C$1</c:f>
+              <c:f>mtcars!$B$1</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -459,12 +463,12 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>mtcars!$B$2:$B$33</c:f>
+              <c:f>mtcars!$C$2:$C$33</c:f>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>mtcars!$C$2:$C$33</c:f>
+              <c:f>mtcars!$B$2:$B$33</c:f>
               <c:numCache/>
             </c:numRef>
           </c:yVal>
@@ -477,11 +481,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1554239083"/>
-        <c:axId val="197460335"/>
+        <c:axId val="1528503465"/>
+        <c:axId val="546947059"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1554239083"/>
+        <c:axId val="1528503465"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -528,7 +532,7 @@
                     </a:solidFill>
                     <a:latin typeface="Roboto"/>
                   </a:rPr>
-                  <a:t>mpg (y)</a:t>
+                  <a:t>hp</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -556,10 +560,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197460335"/>
+        <c:crossAx val="546947059"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="197460335"/>
+        <c:axId val="546947059"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -606,7 +610,7 @@
                     </a:solidFill>
                     <a:latin typeface="Roboto"/>
                   </a:rPr>
-                  <a:t>hp (x)</a:t>
+                  <a:t>mpg</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -634,7 +638,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1554239083"/>
+        <c:crossAx val="1528503465"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -696,13 +700,18 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.71"/>
-    <col customWidth="1" min="2" max="11" width="15.86"/>
-    <col customWidth="1" min="13" max="13" width="17.71"/>
+    <col customWidth="1" min="1" max="1" width="16.38"/>
+    <col customWidth="1" min="2" max="8" width="13.88"/>
+    <col customWidth="1" min="9" max="9" width="22.0"/>
+    <col customWidth="1" min="10" max="11" width="13.88"/>
+    <col customWidth="1" min="13" max="13" width="15.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2582,17 +2591,22 @@
         <v>32</v>
       </c>
       <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+      <c r="D42" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="19">
+        <f>D39^2</f>
+        <v>45.45980326</v>
+      </c>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N42" s="23">
         <f>N41^2</f>
@@ -2603,10 +2617,10 @@
       <c r="Q42" s="4"/>
     </row>
     <row r="43">
-      <c r="A43" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="27">
+      <c r="A43" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="28">
         <f>B42-2</f>
         <v>30</v>
       </c>
@@ -2647,7 +2661,7 @@
     </row>
     <row r="45">
       <c r="A45" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B45" s="20">
         <v>2.04227245630123</v>

</xml_diff>